<commit_message>
✅ Update data tests
</commit_message>
<xml_diff>
--- a/tests/data/IG_DATOS_GATOS_21NOV2021/IG_MORFOMETRIA_GATOS_21NOV2021.xlsx
+++ b/tests/data/IG_DATOS_GATOS_21NOV2021/IG_MORFOMETRIA_GATOS_21NOV2021.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -116,6 +116,21 @@
   </si>
   <si>
     <t xml:space="preserve">Observaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/Nov/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-01-114-SF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maritza Bello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
   </si>
 </sst>
 </file>
@@ -127,7 +142,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -150,6 +165,12 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -193,7 +214,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -223,6 +244,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -247,15 +276,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="G2" activeCellId="0" sqref="G2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.85"/>
@@ -383,6 +412,44 @@
         <v>30</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="9" t="n">
+        <v>378909</v>
+      </c>
+      <c r="E2" s="9" t="n">
+        <v>3198091</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AE1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>